<commit_message>
condition checker returns dataframe when invoked through script
</commit_message>
<xml_diff>
--- a/test_resource/Pattern_Result.xlsx
+++ b/test_resource/Pattern_Result.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Code</t>
   </si>
@@ -28,53 +29,59 @@
     <t>Uniq ID</t>
   </si>
   <si>
-    <t>/functiondefextractor/test_resource/test_repo/src/CerberusTest.java_testCallMethod</t>
-  </si>
-  <si>
-    <t>/functiondefextractor/test_resource/test_repo/src/CerberusTest.java_testCerebrusWithArguments</t>
-  </si>
-  <si>
-    <t>/functiondefextractor/test_resource/test_repo/src/CerberusTest.java_testCerebruswithOutArguments</t>
-  </si>
-  <si>
-    <t>/functiondefextractor/test_resource/test_repo/src/CerberusTest.java_testCerebruswithWrongArguments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Test
-public void testCallMethod() throws Exception {
-assertEquals(Integer.valueOf(0), new Cerberus().call())
-}
+    <t>C:\Users\320074769\Downloads\My_Repos\Python_Repos\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebruswithOutArguments</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\My_Repos\Python_Repos\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebrusWithArguments</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\My_Repos\Python_Repos\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebruswithWrongArguments</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\My_Repos\Python_Repos\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCallMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Test_x000D_
+public void testCerebruswithOutArguments() {_x000D_
+Cerberus.main(new String[] {})_x000D_
+String expectedOutputString = getCerberusCommandLineUsageString()_x000D_
+assertEquals(expectedOutputString, getModifiedOutputStream().toString())_x000D_
+}_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">@Test
-public void testCerebrusWithArguments() {
-getOriginalOutputStream().flush()
-Cerberus.main(new String[] { "CPD" })
-}
+    <t xml:space="preserve">@Test_x000D_
+public void testCerebrusWithArguments() {_x000D_
+getOriginalOutputStream().flush()_x000D_
+Cerberus.main(new String[] { "CPD" })_x000D_
+}_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">@Test
-public void testCerebruswithOutArguments() {
-Cerberus.main(new String[] {})
-String expectedOutputString = getCerberusCommandLineUsageString()
-assertEquals(expectedOutputString, getModifiedOutputStream().toString())
-}
+    <t xml:space="preserve">@Test_x000D_
+public void testCerebruswithWrongArguments() {_x000D_
+String dummyArgument = "dummy argument"_x000D_
+Cerberus.main(new String[] { dummyArgument })_x000D_
+String expectedOutputString = new StringBuilder().append("Unmatched argument at index 0: 'dummy argument'").append(NEW_LINE).append(getCerberusCommandLineUsageString()).toString()_x000D_
+}_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">@Test
-public void testCerebruswithWrongArguments() {
-String dummyArgument = "dummy argument"
-Cerberus.main(new String[] { dummyArgument })
-String expectedOutputString = new StringBuilder().append("Unmatched argument at index 0: 'dummy argument'").append(NEW_LINE).append(getCerberusCommandLineUsageString()).toString()
-}
+    <t xml:space="preserve">@Test_x000D_
+public void testCallMethod() throws Exception {_x000D_
+assertEquals(Integer.valueOf(0), new Cerberus().call())_x000D_
+}_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">@Test
+    <t xml:space="preserve">@Test_x000D_
 </t>
+  </si>
+  <si>
+    <t>Different @Test pattern counts</t>
+  </si>
+  <si>
+    <t>@Test</t>
   </si>
 </sst>
 </file>
@@ -511,4 +518,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>